<commit_message>
Player names being rendered with ng-repeat.
</commit_message>
<xml_diff>
--- a/spurs/players_names_id.xlsx
+++ b/spurs/players_names_id.xlsx
@@ -18,15 +18,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="96">
   <si>
-    <t>Player Id</t>
-  </si>
-  <si>
-    <t>Player First Name</t>
-  </si>
-  <si>
-    <t>Player Last Name</t>
-  </si>
-  <si>
     <t>Yago</t>
   </si>
   <si>
@@ -304,6 +295,15 @@
   </si>
   <si>
     <t>Yedlin</t>
+  </si>
+  <si>
+    <t>Player_Id</t>
+  </si>
+  <si>
+    <t>Player_First_Name</t>
+  </si>
+  <si>
+    <t>Player_Last_Name</t>
   </si>
 </sst>
 </file>
@@ -646,7 +646,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -657,13 +659,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>94</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -671,10 +673,10 @@
         <v>377</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -682,10 +684,10 @@
         <v>378</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -693,10 +695,10 @@
         <v>380</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -704,10 +706,10 @@
         <v>383</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -715,10 +717,10 @@
         <v>388</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -726,10 +728,10 @@
         <v>390</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -737,10 +739,10 @@
         <v>392</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -748,10 +750,10 @@
         <v>395</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -759,10 +761,10 @@
         <v>396</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -770,10 +772,10 @@
         <v>401</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -781,10 +783,10 @@
         <v>402</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -792,10 +794,10 @@
         <v>404</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -803,10 +805,10 @@
         <v>405</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -814,10 +816,10 @@
         <v>410</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -825,10 +827,10 @@
         <v>411</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -836,10 +838,10 @@
         <v>413</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -847,10 +849,10 @@
         <v>414</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -858,10 +860,10 @@
         <v>415</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -869,10 +871,10 @@
         <v>419</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -880,10 +882,10 @@
         <v>420</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -891,10 +893,10 @@
         <v>421</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -902,10 +904,10 @@
         <v>437</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -913,10 +915,10 @@
         <v>445</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -924,10 +926,10 @@
         <v>448</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -935,10 +937,10 @@
         <v>450</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -946,10 +948,10 @@
         <v>471</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -957,10 +959,10 @@
         <v>485</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -968,10 +970,10 @@
         <v>492</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -979,10 +981,10 @@
         <v>493</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -990,10 +992,10 @@
         <v>495</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1001,10 +1003,10 @@
         <v>496</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1012,10 +1014,10 @@
         <v>508</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1023,10 +1025,10 @@
         <v>514</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1034,10 +1036,10 @@
         <v>516</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1045,10 +1047,10 @@
         <v>519</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1056,10 +1058,10 @@
         <v>521</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1067,10 +1069,10 @@
         <v>523</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1078,10 +1080,10 @@
         <v>525</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1089,10 +1091,10 @@
         <v>527</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1100,10 +1102,10 @@
         <v>528</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1111,10 +1113,10 @@
         <v>530</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1122,10 +1124,10 @@
         <v>532</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1133,10 +1135,10 @@
         <v>533</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1144,10 +1146,10 @@
         <v>534</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1155,10 +1157,10 @@
         <v>535</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1166,10 +1168,10 @@
         <v>538</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1177,10 +1179,10 @@
         <v>539</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1188,10 +1190,10 @@
         <v>541</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1199,10 +1201,10 @@
         <v>545</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1210,10 +1212,10 @@
         <v>546</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1221,10 +1223,10 @@
         <v>559</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>